<commit_message>
create Shared String Table if needed when editing template (#31)
</commit_message>
<xml_diff>
--- a/data/blank.xlsx
+++ b/data/blank.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felipenoris/.julia/v0.6/XLSX/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felipenoris/tmp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDFF4DE4-71EC-874F-9D77-00B827A9BFA2}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C353BCB8-5EC8-0143-BDD3-A1B661DAACD7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{B99038AD-B0A3-4743-9234-46915DEE46E8}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,14 +22,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>A</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -378,19 +370,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E867D8FA-35BC-F94D-B286-783204B9A7E3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>